<commit_message>
Dead compartments excluded from aging
Test script test.py will load up standard-test-data-modded.xlsx, which
shows two examples of aging, one with deaths active for juvenile
prisoners.
Accordingly, there is a limit of population transfer as eventually only
deaths are left.
</commit_message>
<xml_diff>
--- a/optima/standard-test-data-modded.xlsx
+++ b/optima/standard-test-data-modded.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -261,10 +261,13 @@
     <t>SNeg XDR Death Rate (Treated)</t>
   </si>
   <si>
+    <t>Death Rate (Other Causes)</t>
+  </si>
+  <si>
     <t>School Age Children</t>
   </si>
   <si>
-    <t>Adults (General)</t>
+    <t>Adults</t>
   </si>
   <si>
     <t>Juvenile Prisoners</t>
@@ -276,13 +279,10 @@
     <t>SAC</t>
   </si>
   <si>
-    <t>Adults</t>
+    <t>JP</t>
   </si>
   <si>
     <t>AP</t>
-  </si>
-  <si>
-    <t>JP</t>
   </si>
   <si>
     <t>y</t>
@@ -626,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -651,10 +651,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -665,10 +665,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C3">
         <v>18</v>
@@ -679,10 +679,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -693,10 +693,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C5">
         <v>18</v>
@@ -715,7 +715,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,9 +778,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH443"/>
+  <dimension ref="A1:AH449"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A419" workbookViewId="0">
+      <selection activeCell="E449" sqref="E449"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -905,7 +907,7 @@
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B3">
         <f>IF(SUMPRODUCT(--(D3:AH3&lt;&gt;""))=0,0,"N.A.")</f>
@@ -1430,7 +1432,7 @@
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B9">
         <f>IF(SUMPRODUCT(--(D9:AH9&lt;&gt;""))=0,1,"N.A.")</f>
@@ -1955,7 +1957,7 @@
     <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B15">
         <f>IF(SUMPRODUCT(--(D15:AH15&lt;&gt;""))=0,0,"N.A.")</f>
@@ -2480,7 +2482,7 @@
     <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B21">
         <f>IF(SUMPRODUCT(--(D21:AH21&lt;&gt;""))=0,1,"N.A.")</f>
@@ -3005,7 +3007,7 @@
     <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B27">
         <f>IF(SUMPRODUCT(--(D27:AH27&lt;&gt;""))=0,0,"N.A.")</f>
@@ -3530,7 +3532,7 @@
     <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B33">
         <f>IF(SUMPRODUCT(--(D33:AH33&lt;&gt;""))=0,1,"N.A.")</f>
@@ -4055,7 +4057,7 @@
     <row r="39" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B39">
         <f>IF(SUMPRODUCT(--(D39:AH39&lt;&gt;""))=0,0,"N.A.")</f>
@@ -4580,7 +4582,7 @@
     <row r="45" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B45">
         <f>IF(SUMPRODUCT(--(D45:AH45&lt;&gt;""))=0,0,"N.A.")</f>
@@ -5105,7 +5107,7 @@
     <row r="51" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B51">
         <f>IF(SUMPRODUCT(--(D51:AH51&lt;&gt;""))=0,0,"N.A.")</f>
@@ -5630,7 +5632,7 @@
     <row r="57" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A57" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B57">
         <f>IF(SUMPRODUCT(--(D57:AH57&lt;&gt;""))=0,0,"N.A.")</f>
@@ -6155,7 +6157,7 @@
     <row r="63" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A63" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B63">
         <f>IF(SUMPRODUCT(--(D63:AH63&lt;&gt;""))=0,0,"N.A.")</f>
@@ -6680,7 +6682,7 @@
     <row r="69" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A69" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B69">
         <f>IF(SUMPRODUCT(--(D69:AH69&lt;&gt;""))=0,0,"N.A.")</f>
@@ -7205,7 +7207,7 @@
     <row r="75" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A75" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B75">
         <f>IF(SUMPRODUCT(--(D75:AH75&lt;&gt;""))=0,0,"N.A.")</f>
@@ -7730,7 +7732,7 @@
     <row r="81" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A81" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B81">
         <f>IF(SUMPRODUCT(--(D81:AH81&lt;&gt;""))=0,0,"N.A.")</f>
@@ -8255,7 +8257,7 @@
     <row r="87" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A87" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B87">
         <f>IF(SUMPRODUCT(--(D87:AH87&lt;&gt;""))=0,0,"N.A.")</f>
@@ -8780,7 +8782,7 @@
     <row r="93" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A93" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B93">
         <f>IF(SUMPRODUCT(--(D93:AH93&lt;&gt;""))=0,0,"N.A.")</f>
@@ -9305,7 +9307,7 @@
     <row r="99" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A99" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B99">
         <f>IF(SUMPRODUCT(--(D99:AH99&lt;&gt;""))=0,0,"N.A.")</f>
@@ -9830,7 +9832,7 @@
     <row r="105" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A105" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B105">
         <f>IF(SUMPRODUCT(--(D105:AH105&lt;&gt;""))=0,1,"N.A.")</f>
@@ -10355,7 +10357,7 @@
     <row r="111" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A111" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B111">
         <f>IF(SUMPRODUCT(--(D111:AH111&lt;&gt;""))=0,0,"N.A.")</f>
@@ -10880,7 +10882,7 @@
     <row r="117" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A117" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B117">
         <f>IF(SUMPRODUCT(--(D117:AH117&lt;&gt;""))=0,0,"N.A.")</f>
@@ -11405,7 +11407,7 @@
     <row r="123" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A123" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B123">
         <f>IF(SUMPRODUCT(--(D123:AH123&lt;&gt;""))=0,0,"N.A.")</f>
@@ -11930,7 +11932,7 @@
     <row r="129" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A129" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B129">
         <f>IF(SUMPRODUCT(--(D129:AH129&lt;&gt;""))=0,0,"N.A.")</f>
@@ -12455,7 +12457,7 @@
     <row r="135" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A135" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B135">
         <f>IF(SUMPRODUCT(--(D135:AH135&lt;&gt;""))=0,0,"N.A.")</f>
@@ -12980,7 +12982,7 @@
     <row r="141" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A141" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B141">
         <f>IF(SUMPRODUCT(--(D141:AH141&lt;&gt;""))=0,0,"N.A.")</f>
@@ -13505,7 +13507,7 @@
     <row r="147" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A147" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B147">
         <f>IF(SUMPRODUCT(--(D147:AH147&lt;&gt;""))=0,0,"N.A.")</f>
@@ -14030,7 +14032,7 @@
     <row r="153" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A153" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B153">
         <f>IF(SUMPRODUCT(--(D153:AH153&lt;&gt;""))=0,0,"N.A.")</f>
@@ -14555,7 +14557,7 @@
     <row r="159" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A159" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B159">
         <f>IF(SUMPRODUCT(--(D159:AH159&lt;&gt;""))=0,1,"N.A.")</f>
@@ -15080,7 +15082,7 @@
     <row r="165" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A165" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B165">
         <f>IF(SUMPRODUCT(--(D165:AH165&lt;&gt;""))=0,0,"N.A.")</f>
@@ -15605,7 +15607,7 @@
     <row r="171" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A171" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B171">
         <f>IF(SUMPRODUCT(--(D171:AH171&lt;&gt;""))=0,0,"N.A.")</f>
@@ -16130,7 +16132,7 @@
     <row r="177" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A177" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B177">
         <f>IF(SUMPRODUCT(--(D177:AH177&lt;&gt;""))=0,1,"N.A.")</f>
@@ -16270,8 +16272,7 @@
         <v>Juvenile Prisoners</v>
       </c>
       <c r="B178">
-        <f>IF(SUMPRODUCT(--(D178:AH178&lt;&gt;""))=0,1,"N.A.")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C178" t="s">
         <v>7</v>
@@ -16655,7 +16656,7 @@
     <row r="183" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A183" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B183">
         <f>IF(SUMPRODUCT(--(D183:AH183&lt;&gt;""))=0,1,"N.A.")</f>
@@ -16795,8 +16796,7 @@
         <v>Juvenile Prisoners</v>
       </c>
       <c r="B184">
-        <f>IF(SUMPRODUCT(--(D184:AH184&lt;&gt;""))=0,1,"N.A.")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C184" t="s">
         <v>7</v>
@@ -17180,7 +17180,7 @@
     <row r="189" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A189" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B189">
         <f>IF(SUMPRODUCT(--(D189:AH189&lt;&gt;""))=0,0,"N.A.")</f>
@@ -17705,7 +17705,7 @@
     <row r="195" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A195" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B195">
         <f>IF(SUMPRODUCT(--(D195:AH195&lt;&gt;""))=0,1,"N.A.")</f>
@@ -18230,7 +18230,7 @@
     <row r="201" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A201" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B201">
         <f>IF(SUMPRODUCT(--(D201:AH201&lt;&gt;""))=0,0,"N.A.")</f>
@@ -18755,7 +18755,7 @@
     <row r="207" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A207" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B207">
         <f>IF(SUMPRODUCT(--(D207:AH207&lt;&gt;""))=0,0,"N.A.")</f>
@@ -19280,7 +19280,7 @@
     <row r="213" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A213" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B213">
         <f>IF(SUMPRODUCT(--(D213:AH213&lt;&gt;""))=0,0,"N.A.")</f>
@@ -19805,7 +19805,7 @@
     <row r="219" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A219" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B219">
         <f>IF(SUMPRODUCT(--(D219:AH219&lt;&gt;""))=0,0,"N.A.")</f>
@@ -20330,7 +20330,7 @@
     <row r="225" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A225" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B225">
         <f>IF(SUMPRODUCT(--(D225:AH225&lt;&gt;""))=0,0,"N.A.")</f>
@@ -20855,7 +20855,7 @@
     <row r="231" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A231" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B231">
         <f>IF(SUMPRODUCT(--(D231:AH231&lt;&gt;""))=0,0,"N.A.")</f>
@@ -21380,7 +21380,7 @@
     <row r="237" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A237" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B237">
         <f>IF(SUMPRODUCT(--(D237:AH237&lt;&gt;""))=0,0,"N.A.")</f>
@@ -21905,7 +21905,7 @@
     <row r="243" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A243" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B243">
         <f>IF(SUMPRODUCT(--(D243:AH243&lt;&gt;""))=0,0,"N.A.")</f>
@@ -22430,7 +22430,7 @@
     <row r="249" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A249" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B249">
         <f>IF(SUMPRODUCT(--(D249:AH249&lt;&gt;""))=0,0,"N.A.")</f>
@@ -22570,8 +22570,7 @@
         <v>Juvenile Prisoners</v>
       </c>
       <c r="B250">
-        <f>IF(SUMPRODUCT(--(D250:AH250&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C250" t="s">
         <v>7</v>
@@ -22955,7 +22954,7 @@
     <row r="255" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A255" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B255">
         <f>IF(SUMPRODUCT(--(D255:AH255&lt;&gt;""))=0,0,"N.A.")</f>
@@ -23480,7 +23479,7 @@
     <row r="261" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A261" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B261">
         <f>IF(SUMPRODUCT(--(D261:AH261&lt;&gt;""))=0,0,"N.A.")</f>
@@ -24005,7 +24004,7 @@
     <row r="267" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A267" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B267">
         <f>IF(SUMPRODUCT(--(D267:AH267&lt;&gt;""))=0,0,"N.A.")</f>
@@ -24530,7 +24529,7 @@
     <row r="273" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A273" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B273">
         <f>IF(SUMPRODUCT(--(D273:AH273&lt;&gt;""))=0,0,"N.A.")</f>
@@ -25055,7 +25054,7 @@
     <row r="279" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A279" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B279">
         <f>IF(SUMPRODUCT(--(D279:AH279&lt;&gt;""))=0,0,"N.A.")</f>
@@ -25580,7 +25579,7 @@
     <row r="285" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A285" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B285">
         <f>IF(SUMPRODUCT(--(D285:AH285&lt;&gt;""))=0,0,"N.A.")</f>
@@ -26105,7 +26104,7 @@
     <row r="291" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A291" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B291">
         <f>IF(SUMPRODUCT(--(D291:AH291&lt;&gt;""))=0,0,"N.A.")</f>
@@ -26630,7 +26629,7 @@
     <row r="297" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A297" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B297">
         <f>IF(SUMPRODUCT(--(D297:AH297&lt;&gt;""))=0,0,"N.A.")</f>
@@ -27155,7 +27154,7 @@
     <row r="303" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A303" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B303">
         <f>IF(SUMPRODUCT(--(D303:AH303&lt;&gt;""))=0,0,"N.A.")</f>
@@ -27680,7 +27679,7 @@
     <row r="309" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A309" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B309">
         <f>IF(SUMPRODUCT(--(D309:AH309&lt;&gt;""))=0,0,"N.A.")</f>
@@ -28205,7 +28204,7 @@
     <row r="315" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A315" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B315">
         <f>IF(SUMPRODUCT(--(D315:AH315&lt;&gt;""))=0,0,"N.A.")</f>
@@ -28730,7 +28729,7 @@
     <row r="321" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A321" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B321">
         <f>IF(SUMPRODUCT(--(D321:AH321&lt;&gt;""))=0,0,"N.A.")</f>
@@ -29255,7 +29254,7 @@
     <row r="327" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A327" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B327">
         <f>IF(SUMPRODUCT(--(D327:AH327&lt;&gt;""))=0,0,"N.A.")</f>
@@ -29780,7 +29779,7 @@
     <row r="333" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A333" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B333">
         <f>IF(SUMPRODUCT(--(D333:AH333&lt;&gt;""))=0,0,"N.A.")</f>
@@ -30305,7 +30304,7 @@
     <row r="339" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A339" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B339">
         <f>IF(SUMPRODUCT(--(D339:AH339&lt;&gt;""))=0,0,"N.A.")</f>
@@ -30830,7 +30829,7 @@
     <row r="345" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A345" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B345">
         <f>IF(SUMPRODUCT(--(D345:AH345&lt;&gt;""))=0,0,"N.A.")</f>
@@ -31355,7 +31354,7 @@
     <row r="351" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A351" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B351">
         <f>IF(SUMPRODUCT(--(D351:AH351&lt;&gt;""))=0,0,"N.A.")</f>
@@ -31880,7 +31879,7 @@
     <row r="357" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A357" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B357">
         <f>IF(SUMPRODUCT(--(D357:AH357&lt;&gt;""))=0,0,"N.A.")</f>
@@ -32405,7 +32404,7 @@
     <row r="363" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A363" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B363">
         <f>IF(SUMPRODUCT(--(D363:AH363&lt;&gt;""))=0,0,"N.A.")</f>
@@ -32930,7 +32929,7 @@
     <row r="369" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A369" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B369">
         <f>IF(SUMPRODUCT(--(D369:AH369&lt;&gt;""))=0,0,"N.A.")</f>
@@ -33455,7 +33454,7 @@
     <row r="375" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A375" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B375">
         <f>IF(SUMPRODUCT(--(D375:AH375&lt;&gt;""))=0,0,"N.A.")</f>
@@ -33980,7 +33979,7 @@
     <row r="381" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A381" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B381">
         <f>IF(SUMPRODUCT(--(D381:AH381&lt;&gt;""))=0,0,"N.A.")</f>
@@ -34505,7 +34504,7 @@
     <row r="387" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A387" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B387">
         <f>IF(SUMPRODUCT(--(D387:AH387&lt;&gt;""))=0,0,"N.A.")</f>
@@ -35030,7 +35029,7 @@
     <row r="393" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A393" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B393">
         <f>IF(SUMPRODUCT(--(D393:AH393&lt;&gt;""))=0,0,"N.A.")</f>
@@ -35555,7 +35554,7 @@
     <row r="399" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A399" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B399">
         <f>IF(SUMPRODUCT(--(D399:AH399&lt;&gt;""))=0,0,"N.A.")</f>
@@ -36080,7 +36079,7 @@
     <row r="405" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A405" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B405">
         <f>IF(SUMPRODUCT(--(D405:AH405&lt;&gt;""))=0,0,"N.A.")</f>
@@ -36605,7 +36604,7 @@
     <row r="411" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A411" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B411">
         <f>IF(SUMPRODUCT(--(D411:AH411&lt;&gt;""))=0,0,"N.A.")</f>
@@ -37130,7 +37129,7 @@
     <row r="417" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A417" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B417">
         <f>IF(SUMPRODUCT(--(D417:AH417&lt;&gt;""))=0,0,"N.A.")</f>
@@ -37655,7 +37654,7 @@
     <row r="423" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A423" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B423">
         <f>IF(SUMPRODUCT(--(D423:AH423&lt;&gt;""))=0,0,"N.A.")</f>
@@ -38180,7 +38179,7 @@
     <row r="429" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A429" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B429">
         <f>IF(SUMPRODUCT(--(D429:AH429&lt;&gt;""))=0,0,"N.A.")</f>
@@ -38705,7 +38704,7 @@
     <row r="435" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A435" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B435">
         <f>IF(SUMPRODUCT(--(D435:AH435&lt;&gt;""))=0,0,"N.A.")</f>
@@ -39230,7 +39229,7 @@
     <row r="441" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A441" t="str">
         <f>'Population Definitions'!A3</f>
-        <v>Adults (General)</v>
+        <v>Adults</v>
       </c>
       <c r="B441">
         <f>IF(SUMPRODUCT(--(D441:AH441&lt;&gt;""))=0,0,"N.A.")</f>
@@ -39638,6 +39637,530 @@
         <v/>
       </c>
     </row>
+    <row r="445" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A445" t="s">
+        <v>81</v>
+      </c>
+      <c r="B445" t="s">
+        <v>6</v>
+      </c>
+      <c r="D445">
+        <v>2000</v>
+      </c>
+      <c r="E445">
+        <v>2001</v>
+      </c>
+      <c r="F445">
+        <v>2002</v>
+      </c>
+      <c r="G445">
+        <v>2003</v>
+      </c>
+      <c r="H445">
+        <v>2004</v>
+      </c>
+      <c r="I445">
+        <v>2005</v>
+      </c>
+      <c r="J445">
+        <v>2006</v>
+      </c>
+      <c r="K445">
+        <v>2007</v>
+      </c>
+      <c r="L445">
+        <v>2008</v>
+      </c>
+      <c r="M445">
+        <v>2009</v>
+      </c>
+      <c r="N445">
+        <v>2010</v>
+      </c>
+      <c r="O445">
+        <v>2011</v>
+      </c>
+      <c r="P445">
+        <v>2012</v>
+      </c>
+      <c r="Q445">
+        <v>2013</v>
+      </c>
+      <c r="R445">
+        <v>2014</v>
+      </c>
+      <c r="S445">
+        <v>2015</v>
+      </c>
+      <c r="T445">
+        <v>2016</v>
+      </c>
+      <c r="U445">
+        <v>2017</v>
+      </c>
+      <c r="V445">
+        <v>2018</v>
+      </c>
+      <c r="W445">
+        <v>2019</v>
+      </c>
+      <c r="X445">
+        <v>2020</v>
+      </c>
+      <c r="Y445">
+        <v>2021</v>
+      </c>
+      <c r="Z445">
+        <v>2022</v>
+      </c>
+      <c r="AA445">
+        <v>2023</v>
+      </c>
+      <c r="AB445">
+        <v>2024</v>
+      </c>
+      <c r="AC445">
+        <v>2025</v>
+      </c>
+      <c r="AD445">
+        <v>2026</v>
+      </c>
+      <c r="AE445">
+        <v>2027</v>
+      </c>
+      <c r="AF445">
+        <v>2028</v>
+      </c>
+      <c r="AG445">
+        <v>2029</v>
+      </c>
+      <c r="AH445">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="446" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A446" t="str">
+        <f>'Population Definitions'!A2</f>
+        <v>School Age Children</v>
+      </c>
+      <c r="B446">
+        <f>IF(SUMPRODUCT(--(D446:AH446&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="C446" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="447" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A447" t="str">
+        <f>'Population Definitions'!A3</f>
+        <v>Adults</v>
+      </c>
+      <c r="B447">
+        <f>IF(SUMPRODUCT(--(D447:AH447&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="C447" t="s">
+        <v>7</v>
+      </c>
+      <c r="D447" t="str">
+        <f t="shared" ref="D447:AH447" si="222">IF(D446="","",D446)</f>
+        <v/>
+      </c>
+      <c r="E447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="F447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="G447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="H447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="I447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="J447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="K447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="L447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="M447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="N447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="O447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="P447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="Q447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="R447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="S447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="T447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="U447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="V447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="W447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="X447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="Y447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="Z447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="AA447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="AB447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="AC447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="AD447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="AE447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="AF447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="AG447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+      <c r="AH447" t="str">
+        <f t="shared" si="222"/>
+        <v/>
+      </c>
+    </row>
+    <row r="448" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A448" t="str">
+        <f>'Population Definitions'!A4</f>
+        <v>Juvenile Prisoners</v>
+      </c>
+      <c r="B448">
+        <v>0.25</v>
+      </c>
+      <c r="C448" t="s">
+        <v>7</v>
+      </c>
+      <c r="D448" t="str">
+        <f t="shared" ref="D448:AH448" si="223">IF(D446="","",D446)</f>
+        <v/>
+      </c>
+      <c r="E448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="F448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="G448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="H448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="I448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="J448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="K448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="L448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="M448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="N448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="O448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="P448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="Q448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="R448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="S448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="T448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="U448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="V448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="W448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="X448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="Y448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="Z448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="AA448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="AB448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="AC448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="AD448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="AE448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="AF448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="AG448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+      <c r="AH448" t="str">
+        <f t="shared" si="223"/>
+        <v/>
+      </c>
+    </row>
+    <row r="449" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A449" t="str">
+        <f>'Population Definitions'!A5</f>
+        <v>Adult Prisoners</v>
+      </c>
+      <c r="B449">
+        <f>IF(SUMPRODUCT(--(D449:AH449&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="C449" t="s">
+        <v>7</v>
+      </c>
+      <c r="D449" t="str">
+        <f t="shared" ref="D449:AH449" si="224">IF(D446="","",D446)</f>
+        <v/>
+      </c>
+      <c r="E449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="F449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="G449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="H449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="I449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="J449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="K449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="L449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="M449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="N449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="O449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="P449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="Q449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="R449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="S449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="T449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="U449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="V449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="W449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="X449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="Y449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="Z449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="AA449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="AB449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="AC449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="AD449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="AE449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="AF449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="AG449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+      <c r="AH449" t="str">
+        <f t="shared" si="224"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>